<commit_message>
Most up to date version. Need to assign roles still.
</commit_message>
<xml_diff>
--- a/Quadratic_Solver_Stories.xlsx
+++ b/Quadratic_Solver_Stories.xlsx
@@ -454,7 +454,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -497,7 +497,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -514,7 +514,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current version of stories. Roles have been assigned.
</commit_message>
<xml_diff>
--- a/Quadratic_Solver_Stories.xlsx
+++ b/Quadratic_Solver_Stories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Tasks</t>
   </si>
@@ -45,9 +45,6 @@
     <t>30 min</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Divide by Zero Error Prevention</t>
   </si>
   <si>
@@ -73,16 +70,54 @@
   </si>
   <si>
     <t>Severity (1-5)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Nick, Brandon, Skylar</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Skylar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,14 +149,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,14 +498,14 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
@@ -474,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -499,66 +543,132 @@
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stories and TPS report for this week
</commit_message>
<xml_diff>
--- a/Quadratic_Solver_Stories.xlsx
+++ b/Quadratic_Solver_Stories.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6080" yWindow="440" windowWidth="25040" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,111 +19,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
-  <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Assigned</t>
-  </si>
-  <si>
-    <t>Actual Time</t>
-  </si>
-  <si>
-    <t>Code Completed</t>
-  </si>
-  <si>
-    <t>Code Review/Analysis</t>
-  </si>
-  <si>
-    <t>Research IEEE Floating Point</t>
-  </si>
-  <si>
-    <t>30 min</t>
-  </si>
-  <si>
-    <t>Divide by Zero Error Prevention</t>
-  </si>
-  <si>
-    <t>10 min</t>
-  </si>
-  <si>
-    <t>NaN's and INF's Error Prevention</t>
-  </si>
-  <si>
-    <t>Memory Leak Prevention</t>
-  </si>
-  <si>
-    <t>15 min</t>
-  </si>
-  <si>
-    <t>Square Root Function Implementation</t>
-  </si>
-  <si>
-    <t>Quadratic Solver Implementation</t>
-  </si>
-  <si>
-    <t>1.5 hours</t>
-  </si>
-  <si>
-    <t>Severity (1-5)</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Nick, Brandon, Skylar</t>
-  </si>
-  <si>
-    <t>Brandon</t>
-  </si>
-  <si>
-    <t>Nick</t>
-  </si>
-  <si>
-    <t>Skylar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Time To Complete</t>
+  </si>
+  <si>
+    <t>Risk (1-5)</t>
+  </si>
+  <si>
+    <t>Prompt User to Input three values</t>
+  </si>
+  <si>
+    <t>Allow input to handle more than integer values</t>
+  </si>
+  <si>
+    <t>Implement NaN's and INF's Error Prevention</t>
+  </si>
+  <si>
+    <t>Do IEEE computations in double precision</t>
+  </si>
+  <si>
+    <t>Output the result to the user in IEEE single precision</t>
+  </si>
+  <si>
+    <t>Create test cases to test each individual module</t>
+  </si>
+  <si>
+    <t>Allow program to be ran using a MakeFile</t>
+  </si>
+  <si>
+    <t>Allow program to be compatible with GCC and Linux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,35 +93,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,22 +430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,163 +450,99 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4">
+        <v>0</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>